<commit_message>
se solucionaron errores, ahora al scanear un codigo que ya cuenta con un registro solo imprime el mensaje de aviso
</commit_message>
<xml_diff>
--- a/2024-12-16.xlsx
+++ b/2024-12-16.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,17 +443,48 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>FECHA</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>HORA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>G101</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>E102</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>S104</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-12-16</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>11:51:27</t>
         </is>
       </c>
     </row>

</xml_diff>